<commit_message>
Update American option tree example
</commit_message>
<xml_diff>
--- a/CoxRossRubinsteinModel/AmericanOptionTree.xlsx
+++ b/CoxRossRubinsteinModel/AmericanOptionTree.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="European Option" sheetId="1" r:id="rId1"/>
+    <sheet name="American Option" sheetId="1" r:id="rId1"/>
+    <sheet name="American Option (empty)" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
   <si>
     <t>r</t>
   </si>
@@ -658,7 +659,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B3:R58"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
@@ -799,43 +802,43 @@
         <v>1</v>
       </c>
       <c r="D18" s="16">
-        <f>C18*(1+$C$10)</f>
+        <f t="shared" ref="D18:M18" si="0">C18*(1+$C$10)</f>
         <v>1.0693832060523671</v>
       </c>
       <c r="E18" s="16">
-        <f>D18*(1+$C$10)</f>
+        <f t="shared" si="0"/>
         <v>1.1435804413868396</v>
       </c>
       <c r="F18" s="16">
-        <f>E18*(1+$C$10)</f>
+        <f t="shared" si="0"/>
         <v>1.2229257187890397</v>
       </c>
       <c r="G18" s="16">
-        <f>F18*(1+$C$10)</f>
+        <f t="shared" si="0"/>
         <v>1.3077762259225187</v>
       </c>
       <c r="H18" s="16">
-        <f>G18*(1+$C$10)</f>
+        <f t="shared" si="0"/>
         <v>1.3985139332760879</v>
       </c>
       <c r="I18" s="16">
-        <f>H18*(1+$C$10)</f>
+        <f t="shared" si="0"/>
         <v>1.4955473136756892</v>
       </c>
       <c r="J18" s="16">
-        <f>I18*(1+$C$10)</f>
+        <f t="shared" si="0"/>
         <v>1.5993131811015135</v>
       </c>
       <c r="K18" s="16">
-        <f>J18*(1+$C$10)</f>
+        <f t="shared" si="0"/>
         <v>1.7102786570881465</v>
       </c>
       <c r="L18" s="16">
-        <f>K18*(1+$C$10)</f>
+        <f t="shared" si="0"/>
         <v>1.8289432735598592</v>
       </c>
       <c r="M18" s="17">
-        <f>L18*(1+$C$10)</f>
+        <f t="shared" si="0"/>
         <v>1.9558412215673537</v>
       </c>
     </row>
@@ -843,43 +846,43 @@
       <c r="B19" s="25"/>
       <c r="C19" s="18"/>
       <c r="D19" s="19">
-        <f>C18*(1+$C$11)</f>
+        <f t="shared" ref="D19:M19" si="1">C18*(1+$C$11)</f>
         <v>0.93511848170077816</v>
       </c>
       <c r="E19" s="19">
-        <f>D18*(1+$C$11)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="F19" s="19">
-        <f>E18*(1+$C$11)</f>
+        <f t="shared" si="1"/>
         <v>1.0693832060523671</v>
       </c>
       <c r="G19" s="19">
-        <f>F18*(1+$C$11)</f>
+        <f t="shared" si="1"/>
         <v>1.1435804413868396</v>
       </c>
       <c r="H19" s="19">
-        <f>G18*(1+$C$11)</f>
+        <f t="shared" si="1"/>
         <v>1.2229257187890397</v>
       </c>
       <c r="I19" s="19">
-        <f>H18*(1+$C$11)</f>
+        <f t="shared" si="1"/>
         <v>1.3077762259225187</v>
       </c>
       <c r="J19" s="19">
-        <f>I18*(1+$C$11)</f>
+        <f t="shared" si="1"/>
         <v>1.3985139332760879</v>
       </c>
       <c r="K19" s="19">
-        <f>J18*(1+$C$11)</f>
+        <f t="shared" si="1"/>
         <v>1.4955473136756889</v>
       </c>
       <c r="L19" s="19">
-        <f>K18*(1+$C$11)</f>
+        <f t="shared" si="1"/>
         <v>1.5993131811015133</v>
       </c>
       <c r="M19" s="20">
-        <f>L18*(1+$C$11)</f>
+        <f t="shared" si="1"/>
         <v>1.7102786570881465</v>
       </c>
     </row>
@@ -888,39 +891,39 @@
       <c r="C20" s="18"/>
       <c r="D20" s="19"/>
       <c r="E20" s="19">
-        <f>D19*(1+$C$11)</f>
+        <f t="shared" ref="E20:M20" si="2">D19*(1+$C$11)</f>
         <v>0.87444657481836863</v>
       </c>
       <c r="F20" s="19">
-        <f>E19*(1+$C$11)</f>
+        <f t="shared" si="2"/>
         <v>0.93511848170077816</v>
       </c>
       <c r="G20" s="19">
-        <f>F19*(1+$C$11)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H20" s="19">
-        <f>G19*(1+$C$11)</f>
+        <f t="shared" si="2"/>
         <v>1.0693832060523671</v>
       </c>
       <c r="I20" s="19">
-        <f>H19*(1+$C$11)</f>
+        <f t="shared" si="2"/>
         <v>1.1435804413868396</v>
       </c>
       <c r="J20" s="19">
-        <f>I19*(1+$C$11)</f>
+        <f t="shared" si="2"/>
         <v>1.2229257187890397</v>
       </c>
       <c r="K20" s="19">
-        <f>J19*(1+$C$11)</f>
+        <f t="shared" si="2"/>
         <v>1.3077762259225187</v>
       </c>
       <c r="L20" s="19">
-        <f>K19*(1+$C$11)</f>
+        <f t="shared" si="2"/>
         <v>1.3985139332760876</v>
       </c>
       <c r="M20" s="20">
-        <f>L19*(1+$C$11)</f>
+        <f t="shared" si="2"/>
         <v>1.4955473136756887</v>
       </c>
     </row>
@@ -930,35 +933,35 @@
       <c r="D21" s="19"/>
       <c r="E21" s="19"/>
       <c r="F21" s="19">
-        <f>E20*(1+$C$11)</f>
+        <f t="shared" ref="F21:M21" si="3">E20*(1+$C$11)</f>
         <v>0.81771115337259881</v>
       </c>
       <c r="G21" s="19">
-        <f>F20*(1+$C$11)</f>
+        <f t="shared" si="3"/>
         <v>0.87444657481836863</v>
       </c>
       <c r="H21" s="19">
-        <f>G20*(1+$C$11)</f>
+        <f t="shared" si="3"/>
         <v>0.93511848170077816</v>
       </c>
       <c r="I21" s="19">
-        <f>H20*(1+$C$11)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J21" s="19">
-        <f>I20*(1+$C$11)</f>
+        <f t="shared" si="3"/>
         <v>1.0693832060523671</v>
       </c>
       <c r="K21" s="19">
-        <f>J20*(1+$C$11)</f>
+        <f t="shared" si="3"/>
         <v>1.1435804413868396</v>
       </c>
       <c r="L21" s="19">
-        <f>K20*(1+$C$11)</f>
+        <f t="shared" si="3"/>
         <v>1.2229257187890397</v>
       </c>
       <c r="M21" s="20">
-        <f>L20*(1+$C$11)</f>
+        <f t="shared" si="3"/>
         <v>1.3077762259225185</v>
       </c>
     </row>
@@ -969,31 +972,31 @@
       <c r="E22" s="19"/>
       <c r="F22" s="19"/>
       <c r="G22" s="19">
-        <f>F21*(1+$C$11)</f>
+        <f t="shared" ref="G22:M22" si="4">F21*(1+$C$11)</f>
         <v>0.76465681221157678</v>
       </c>
       <c r="H22" s="19">
-        <f>G21*(1+$C$11)</f>
+        <f t="shared" si="4"/>
         <v>0.81771115337259881</v>
       </c>
       <c r="I22" s="19">
-        <f>H21*(1+$C$11)</f>
+        <f t="shared" si="4"/>
         <v>0.87444657481836863</v>
       </c>
       <c r="J22" s="19">
-        <f>I21*(1+$C$11)</f>
+        <f t="shared" si="4"/>
         <v>0.93511848170077816</v>
       </c>
       <c r="K22" s="19">
-        <f>J21*(1+$C$11)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L22" s="19">
-        <f>K21*(1+$C$11)</f>
+        <f t="shared" si="4"/>
         <v>1.0693832060523671</v>
       </c>
       <c r="M22" s="20">
-        <f>L21*(1+$C$11)</f>
+        <f t="shared" si="4"/>
         <v>1.1435804413868396</v>
       </c>
     </row>
@@ -1005,27 +1008,27 @@
       <c r="F23" s="19"/>
       <c r="G23" s="19"/>
       <c r="H23" s="19">
-        <f>G22*(1+$C$11)</f>
+        <f t="shared" ref="H23:M23" si="5">G22*(1+$C$11)</f>
         <v>0.71504471725744667</v>
       </c>
       <c r="I23" s="19">
-        <f>H22*(1+$C$11)</f>
+        <f t="shared" si="5"/>
         <v>0.76465681221157678</v>
       </c>
       <c r="J23" s="19">
-        <f>I22*(1+$C$11)</f>
+        <f t="shared" si="5"/>
         <v>0.81771115337259881</v>
       </c>
       <c r="K23" s="19">
-        <f>J22*(1+$C$11)</f>
+        <f t="shared" si="5"/>
         <v>0.87444657481836863</v>
       </c>
       <c r="L23" s="19">
-        <f>K22*(1+$C$11)</f>
+        <f t="shared" si="5"/>
         <v>0.93511848170077816</v>
       </c>
       <c r="M23" s="20">
-        <f>L22*(1+$C$11)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="R23" s="31"/>
@@ -1180,47 +1183,47 @@
         <v>19</v>
       </c>
       <c r="C34" s="15">
-        <f>MAX($C$30*(C18-$C$31),0)/(1+$C$9)^C$16</f>
+        <f t="shared" ref="C34:M34" si="6">MAX($C$30*(C18-$C$31),0)/(1+$C$9)^C$16</f>
         <v>0</v>
       </c>
       <c r="D34" s="16">
-        <f>MAX($C$30*(D18-$C$31),0)/(1+$C$9)^D$16</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E34" s="16">
-        <f>MAX($C$30*(E18-$C$31),0)/(1+$C$9)^E$16</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F34" s="16">
-        <f>MAX($C$30*(F18-$C$31),0)/(1+$C$9)^F$16</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G34" s="16">
-        <f>MAX($C$30*(G18-$C$31),0)/(1+$C$9)^G$16</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H34" s="16">
-        <f>MAX($C$30*(H18-$C$31),0)/(1+$C$9)^H$16</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I34" s="16">
-        <f>MAX($C$30*(I18-$C$31),0)/(1+$C$9)^I$16</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J34" s="16">
-        <f>MAX($C$30*(J18-$C$31),0)/(1+$C$9)^J$16</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K34" s="16">
-        <f>MAX($C$30*(K18-$C$31),0)/(1+$C$9)^K$16</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="L34" s="16">
-        <f>MAX($C$30*(L18-$C$31),0)/(1+$C$9)^L$16</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M34" s="17">
-        <f>MAX($C$30*(M18-$C$31),0)/(1+$C$9)^M$16</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -1228,43 +1231,43 @@
       <c r="B35" s="25"/>
       <c r="C35" s="18"/>
       <c r="D35" s="19">
-        <f>MAX($C$30*(D19-$C$31),0)/(1+$C$9)^D$16</f>
+        <f t="shared" ref="D35:M35" si="7">MAX($C$30*(D19-$C$31),0)/(1+$C$9)^D$16</f>
         <v>6.4493394724520633E-2</v>
       </c>
       <c r="E35" s="19">
-        <f>MAX($C$30*(E19-$C$31),0)/(1+$C$9)^E$16</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F35" s="19">
-        <f>MAX($C$30*(F19-$C$31),0)/(1+$C$9)^F$16</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G35" s="19">
-        <f>MAX($C$30*(G19-$C$31),0)/(1+$C$9)^G$16</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H35" s="19">
-        <f>MAX($C$30*(H19-$C$31),0)/(1+$C$9)^H$16</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I35" s="19">
-        <f>MAX($C$30*(I19-$C$31),0)/(1+$C$9)^I$16</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J35" s="19">
-        <f>MAX($C$30*(J19-$C$31),0)/(1+$C$9)^J$16</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K35" s="19">
-        <f>MAX($C$30*(K19-$C$31),0)/(1+$C$9)^K$16</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L35" s="19">
-        <f>MAX($C$30*(L19-$C$31),0)/(1+$C$9)^L$16</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M35" s="20">
-        <f>MAX($C$30*(M19-$C$31),0)/(1+$C$9)^M$16</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -1273,39 +1276,39 @@
       <c r="C36" s="18"/>
       <c r="D36" s="19"/>
       <c r="E36" s="19">
-        <f>MAX($C$30*(E20-$C$31),0)/(1+$C$9)^E$16</f>
+        <f t="shared" ref="E36:M36" si="8">MAX($C$30*(E20-$C$31),0)/(1+$C$9)^E$16</f>
         <v>0.12405578787489675</v>
       </c>
       <c r="F36" s="19">
-        <f>MAX($C$30*(F20-$C$31),0)/(1+$C$9)^F$16</f>
+        <f t="shared" si="8"/>
         <v>6.3724098993737696E-2</v>
       </c>
       <c r="G36" s="19">
-        <f>MAX($C$30*(G20-$C$31),0)/(1+$C$9)^G$16</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="H36" s="19">
-        <f>MAX($C$30*(H20-$C$31),0)/(1+$C$9)^H$16</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I36" s="19">
-        <f>MAX($C$30*(I20-$C$31),0)/(1+$C$9)^I$16</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J36" s="19">
-        <f>MAX($C$30*(J20-$C$31),0)/(1+$C$9)^J$16</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K36" s="19">
-        <f>MAX($C$30*(K20-$C$31),0)/(1+$C$9)^K$16</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L36" s="19">
-        <f>MAX($C$30*(L20-$C$31),0)/(1+$C$9)^L$16</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="M36" s="20">
-        <f>MAX($C$30*(M20-$C$31),0)/(1+$C$9)^M$16</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -1315,35 +1318,35 @@
       <c r="D37" s="19"/>
       <c r="E37" s="19"/>
       <c r="F37" s="19">
-        <f>MAX($C$30*(F21-$C$31),0)/(1+$C$9)^F$16</f>
+        <f t="shared" ref="F37:M37" si="9">MAX($C$30*(F21-$C$31),0)/(1+$C$9)^F$16</f>
         <v>0.17903700179097226</v>
       </c>
       <c r="G37" s="19">
-        <f>MAX($C$30*(G21-$C$31),0)/(1+$C$9)^G$16</f>
+        <f t="shared" si="9"/>
         <v>0.12257601481598553</v>
       </c>
       <c r="H37" s="19">
-        <f>MAX($C$30*(H21-$C$31),0)/(1+$C$9)^H$16</f>
+        <f t="shared" si="9"/>
         <v>6.2963979643325618E-2</v>
       </c>
       <c r="I37" s="19">
-        <f>MAX($C$30*(I21-$C$31),0)/(1+$C$9)^I$16</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J37" s="19">
-        <f>MAX($C$30*(J21-$C$31),0)/(1+$C$9)^J$16</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="K37" s="19">
-        <f>MAX($C$30*(K21-$C$31),0)/(1+$C$9)^K$16</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="L37" s="19">
-        <f>MAX($C$30*(L21-$C$31),0)/(1+$C$9)^L$16</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M37" s="20">
-        <f>MAX($C$30*(M21-$C$31),0)/(1+$C$9)^M$16</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -1354,31 +1357,31 @@
       <c r="E38" s="19"/>
       <c r="F38" s="19"/>
       <c r="G38" s="19">
-        <f>MAX($C$30*(G22-$C$31),0)/(1+$C$9)^G$16</f>
+        <f t="shared" ref="G38:M38" si="10">MAX($C$30*(G22-$C$31),0)/(1+$C$9)^G$16</f>
         <v>0.22976219112670965</v>
       </c>
       <c r="H38" s="19">
-        <f>MAX($C$30*(H22-$C$31),0)/(1+$C$9)^H$16</f>
+        <f t="shared" si="10"/>
         <v>0.17690139702527047</v>
       </c>
       <c r="I38" s="19">
-        <f>MAX($C$30*(I22-$C$31),0)/(1+$C$9)^I$16</f>
+        <f t="shared" si="10"/>
         <v>0.1211138929150202</v>
       </c>
       <c r="J38" s="19">
-        <f>MAX($C$30*(J22-$C$31),0)/(1+$C$9)^J$16</f>
+        <f t="shared" si="10"/>
         <v>6.2212927214784462E-2</v>
       </c>
       <c r="K38" s="19">
-        <f>MAX($C$30*(K22-$C$31),0)/(1+$C$9)^K$16</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="L38" s="19">
-        <f>MAX($C$30*(L22-$C$31),0)/(1+$C$9)^L$16</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="M38" s="20">
-        <f>MAX($C$30*(M22-$C$31),0)/(1+$C$9)^M$16</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -1390,27 +1393,27 @@
       <c r="F39" s="19"/>
       <c r="G39" s="19"/>
       <c r="H39" s="19">
-        <f>MAX($C$30*(H23-$C$31),0)/(1+$C$9)^H$16</f>
+        <f t="shared" ref="H39:M39" si="11">MAX($C$30*(H23-$C$31),0)/(1+$C$9)^H$16</f>
         <v>0.2765335813985631</v>
       </c>
       <c r="I39" s="19">
-        <f>MAX($C$30*(I23-$C$31),0)/(1+$C$9)^I$16</f>
+        <f t="shared" si="11"/>
         <v>0.22702152173747828</v>
       </c>
       <c r="J39" s="19">
-        <f>MAX($C$30*(J23-$C$31),0)/(1+$C$9)^J$16</f>
+        <f t="shared" si="11"/>
         <v>0.17479126636642739</v>
       </c>
       <c r="K39" s="19">
-        <f>MAX($C$30*(K23-$C$31),0)/(1+$C$9)^K$16</f>
+        <f t="shared" si="11"/>
         <v>0.11966921162392043</v>
       </c>
       <c r="L39" s="19">
-        <f>MAX($C$30*(L23-$C$31),0)/(1+$C$9)^L$16</f>
+        <f t="shared" si="11"/>
         <v>6.1470833555266703E-2</v>
       </c>
       <c r="M39" s="20">
-        <f>MAX($C$30*(M23-$C$31),0)/(1+$C$9)^M$16</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -1539,43 +1542,43 @@
         <v>9</v>
       </c>
       <c r="C48" s="15">
-        <f>MAX($C$12*D48+(1-$C$12)*D49,C34)</f>
+        <f t="shared" ref="C48:L48" si="12">MAX($C$12*D48+(1-$C$12)*D49,C34)</f>
         <v>6.1569431106759942E-2</v>
       </c>
       <c r="D48" s="16">
-        <f>MAX($C$12*E48+(1-$C$12)*E49,D34)</f>
+        <f t="shared" si="12"/>
         <v>3.5636487895058869E-2</v>
       </c>
       <c r="E48" s="16">
-        <f>MAX($C$12*F48+(1-$C$12)*F49,E34)</f>
+        <f t="shared" si="12"/>
         <v>1.7544440625619183E-2</v>
       </c>
       <c r="F48" s="16">
-        <f>MAX($C$12*G48+(1-$C$12)*G49,F34)</f>
+        <f t="shared" si="12"/>
         <v>6.6015563787102409E-3</v>
       </c>
       <c r="G48" s="16">
-        <f>MAX($C$12*H48+(1-$C$12)*H49,G34)</f>
+        <f t="shared" si="12"/>
         <v>1.4391713379539324E-3</v>
       </c>
       <c r="H48" s="16">
-        <f>MAX($C$12*I48+(1-$C$12)*I49,H34)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="I48" s="16">
-        <f>MAX($C$12*J48+(1-$C$12)*J49,I34)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="J48" s="16">
-        <f>MAX($C$12*K48+(1-$C$12)*K49,J34)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="K48" s="16">
-        <f>MAX($C$12*L48+(1-$C$12)*L49,K34)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="L48" s="16">
-        <f>MAX($C$12*M48+(1-$C$12)*M49,L34)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M48" s="17">
@@ -1587,43 +1590,43 @@
       <c r="B49" s="25"/>
       <c r="C49" s="18"/>
       <c r="D49" s="19">
-        <f t="shared" ref="D49" si="0">MAX($C$12*E49+(1-$C$12)*E50,D35)</f>
+        <f t="shared" ref="D49" si="13">MAX($C$12*E49+(1-$C$12)*E50,D35)</f>
         <v>9.0585909983530291E-2</v>
       </c>
       <c r="E49" s="19">
-        <f t="shared" ref="E49:F49" si="1">MAX($C$12*F49+(1-$C$12)*F50,E35)</f>
+        <f t="shared" ref="E49:F49" si="14">MAX($C$12*F49+(1-$C$12)*F50,E35)</f>
         <v>5.5879755431092318E-2</v>
       </c>
       <c r="F49" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="14"/>
         <v>2.9788479684714798E-2</v>
       </c>
       <c r="G49" s="19">
-        <f t="shared" ref="G49:H49" si="2">MAX($C$12*H49+(1-$C$12)*H50,G35)</f>
+        <f t="shared" ref="G49:H49" si="15">MAX($C$12*H49+(1-$C$12)*H50,G35)</f>
         <v>1.2377770642784704E-2</v>
       </c>
       <c r="H49" s="19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="15"/>
         <v>3.0494661813464646E-3</v>
       </c>
       <c r="I49" s="19">
-        <f t="shared" ref="I49:J49" si="3">MAX($C$12*J49+(1-$C$12)*J50,I35)</f>
+        <f t="shared" ref="I49:J49" si="16">MAX($C$12*J49+(1-$C$12)*J50,I35)</f>
         <v>0</v>
       </c>
       <c r="J49" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="K49" s="19">
-        <f t="shared" ref="K49:L57" si="4">MAX($C$12*L49+(1-$C$12)*L50,K35)</f>
+        <f t="shared" ref="K49:L57" si="17">MAX($C$12*L49+(1-$C$12)*L50,K35)</f>
         <v>0</v>
       </c>
       <c r="L49" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="M49" s="20">
-        <f t="shared" ref="M49:M58" si="5">M35</f>
+        <f t="shared" ref="M49:M58" si="18">M35</f>
         <v>0</v>
       </c>
     </row>
@@ -1632,39 +1635,39 @@
       <c r="C50" s="18"/>
       <c r="D50" s="19"/>
       <c r="E50" s="19">
-        <f t="shared" ref="E50:F50" si="6">MAX($C$12*F50+(1-$C$12)*F51,E36)</f>
+        <f t="shared" ref="E50:F50" si="19">MAX($C$12*F50+(1-$C$12)*F51,E36)</f>
         <v>0.12941877180888445</v>
       </c>
       <c r="F50" s="19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="19"/>
         <v>8.5073393244680606E-2</v>
       </c>
       <c r="G50" s="19">
-        <f t="shared" ref="G50:H50" si="7">MAX($C$12*H50+(1-$C$12)*H51,G36)</f>
+        <f t="shared" ref="G50:H50" si="20">MAX($C$12*H50+(1-$C$12)*H51,G36)</f>
         <v>4.9269395021652403E-2</v>
       </c>
       <c r="H50" s="19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="20"/>
         <v>2.2815249611206446E-2</v>
       </c>
       <c r="I50" s="19">
-        <f t="shared" ref="I50:J50" si="8">MAX($C$12*J50+(1-$C$12)*J51,I36)</f>
+        <f t="shared" ref="I50:J50" si="21">MAX($C$12*J50+(1-$C$12)*J51,I36)</f>
         <v>6.4615266757580853E-3</v>
       </c>
       <c r="J50" s="19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="K50" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="L50" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="M50" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
@@ -1674,35 +1677,35 @@
       <c r="D51" s="19"/>
       <c r="E51" s="19"/>
       <c r="F51" s="19">
-        <f t="shared" ref="F51" si="9">MAX($C$12*G51+(1-$C$12)*G52,F37)</f>
+        <f t="shared" ref="F51" si="22">MAX($C$12*G51+(1-$C$12)*G52,F37)</f>
         <v>0.17903700179097226</v>
       </c>
       <c r="G51" s="19">
-        <f t="shared" ref="G51:H51" si="10">MAX($C$12*H51+(1-$C$12)*H52,G37)</f>
+        <f t="shared" ref="G51:H51" si="23">MAX($C$12*H51+(1-$C$12)*H52,G37)</f>
         <v>0.12513463695548555</v>
       </c>
       <c r="H51" s="19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="23"/>
         <v>7.8869049223604659E-2</v>
       </c>
       <c r="I51" s="19">
-        <f t="shared" ref="I51:J51" si="11">MAX($C$12*J51+(1-$C$12)*J52,I37)</f>
+        <f t="shared" ref="I51:J51" si="24">MAX($C$12*J51+(1-$C$12)*J52,I37)</f>
         <v>4.1113498762459094E-2</v>
       </c>
       <c r="J51" s="19">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>1.3691355961553379E-2</v>
       </c>
       <c r="K51" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="L51" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="M51" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
@@ -1713,31 +1716,31 @@
       <c r="E52" s="19"/>
       <c r="F52" s="19"/>
       <c r="G52" s="19">
-        <f t="shared" ref="G52:H52" si="12">MAX($C$12*H52+(1-$C$12)*H53,G38)</f>
+        <f t="shared" ref="G52:H52" si="25">MAX($C$12*H52+(1-$C$12)*H53,G38)</f>
         <v>0.22976219112670965</v>
       </c>
       <c r="H52" s="19">
-        <f t="shared" si="12"/>
+        <f t="shared" si="25"/>
         <v>0.17690139702527047</v>
       </c>
       <c r="I52" s="19">
-        <f t="shared" ref="I52:J52" si="13">MAX($C$12*J52+(1-$C$12)*J53,I38)</f>
+        <f t="shared" ref="I52:J52" si="26">MAX($C$12*J52+(1-$C$12)*J53,I38)</f>
         <v>0.1211138929150202</v>
       </c>
       <c r="J52" s="19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="26"/>
         <v>7.1796249302676987E-2</v>
       </c>
       <c r="K52" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="17"/>
         <v>2.9010671544425791E-2</v>
       </c>
       <c r="L52" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="M52" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
@@ -1749,27 +1752,27 @@
       <c r="F53" s="19"/>
       <c r="G53" s="19"/>
       <c r="H53" s="19">
-        <f t="shared" ref="H53" si="14">MAX($C$12*I53+(1-$C$12)*I54,H39)</f>
+        <f t="shared" ref="H53" si="27">MAX($C$12*I53+(1-$C$12)*I54,H39)</f>
         <v>0.2765335813985631</v>
       </c>
       <c r="I53" s="19">
-        <f t="shared" ref="I53:J53" si="15">MAX($C$12*J53+(1-$C$12)*J54,I39)</f>
+        <f t="shared" ref="I53:J53" si="28">MAX($C$12*J53+(1-$C$12)*J54,I39)</f>
         <v>0.22702152173747828</v>
       </c>
       <c r="J53" s="19">
-        <f t="shared" si="15"/>
+        <f t="shared" si="28"/>
         <v>0.17479126636642739</v>
       </c>
       <c r="K53" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="17"/>
         <v>0.11966921162392043</v>
       </c>
       <c r="L53" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="17"/>
         <v>6.1470833555266703E-2</v>
       </c>
       <c r="M53" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
     </row>
@@ -1782,23 +1785,23 @@
       <c r="G54" s="19"/>
       <c r="H54" s="19"/>
       <c r="I54" s="19">
-        <f t="shared" ref="I54:J54" si="16">MAX($C$12*J54+(1-$C$12)*J55,I40)</f>
+        <f t="shared" ref="I54:J54" si="29">MAX($C$12*J54+(1-$C$12)*J55,I40)</f>
         <v>0.319632085008412</v>
       </c>
       <c r="J54" s="19">
-        <f t="shared" si="16"/>
+        <f t="shared" si="29"/>
         <v>0.27323500943632228</v>
       </c>
       <c r="K54" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="17"/>
         <v>0.22431354383967211</v>
       </c>
       <c r="L54" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="17"/>
         <v>0.17270630595198189</v>
       </c>
       <c r="M54" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>0.11824176290608389</v>
       </c>
     </row>
@@ -1812,19 +1815,19 @@
       <c r="H55" s="19"/>
       <c r="I55" s="19"/>
       <c r="J55" s="19">
-        <f t="shared" ref="J55" si="17">MAX($C$12*K55+(1-$C$12)*K56,J41)</f>
+        <f t="shared" ref="J55" si="30">MAX($C$12*K55+(1-$C$12)*K56,J41)</f>
         <v>0.35931880337609134</v>
       </c>
       <c r="K55" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="17"/>
         <v>0.31581942171989175</v>
       </c>
       <c r="L55" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="17"/>
         <v>0.26997578378759274</v>
       </c>
       <c r="M55" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>0.22163786747979455</v>
       </c>
     </row>
@@ -1839,15 +1842,15 @@
       <c r="I56" s="19"/>
       <c r="J56" s="19"/>
       <c r="K56" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="17"/>
         <v>0.39583642320799761</v>
       </c>
       <c r="L56" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="17"/>
         <v>0.35503274551531389</v>
       </c>
       <c r="M56" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>0.31205223697383783</v>
       </c>
     </row>
@@ -1863,11 +1866,11 @@
       <c r="J57" s="19"/>
       <c r="K57" s="19"/>
       <c r="L57" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="17"/>
         <v>0.4294105143625766</v>
       </c>
       <c r="M57" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>0.39111477269226619</v>
       </c>
     </row>
@@ -1884,8 +1887,924 @@
       <c r="K58" s="28"/>
       <c r="L58" s="28"/>
       <c r="M58" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>0.46025073624770091</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:R58"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="13" width="9.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="8">
+        <f>EXP(C5*C3/C4)-1</f>
+        <v>6.0180360540649236E-3</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="9">
+        <f>EXP(C6*SQRT(C3/C4))-1</f>
+        <v>6.9383206052367141E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="9">
+        <f>EXP(-C6*SQRT(C3/C4))-1</f>
+        <v>-6.4881518299221841E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="10">
+        <f>(C9-C11)/(C10-C11)</f>
+        <v>0.52805794445030407</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G14" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B16" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="11">
+        <v>0</v>
+      </c>
+      <c r="D16" s="12">
+        <v>1</v>
+      </c>
+      <c r="E16" s="12">
+        <v>2</v>
+      </c>
+      <c r="F16" s="12">
+        <v>3</v>
+      </c>
+      <c r="G16" s="12">
+        <v>4</v>
+      </c>
+      <c r="H16" s="12">
+        <v>5</v>
+      </c>
+      <c r="I16" s="12">
+        <v>6</v>
+      </c>
+      <c r="J16" s="12">
+        <v>7</v>
+      </c>
+      <c r="K16" s="12">
+        <v>8</v>
+      </c>
+      <c r="L16" s="12">
+        <v>9</v>
+      </c>
+      <c r="M16" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B18" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="15">
+        <f>C7</f>
+        <v>1</v>
+      </c>
+      <c r="D18" s="16">
+        <f t="shared" ref="D18:M18" si="0">C18*(1+$C$10)</f>
+        <v>1.0693832060523671</v>
+      </c>
+      <c r="E18" s="16">
+        <f t="shared" si="0"/>
+        <v>1.1435804413868396</v>
+      </c>
+      <c r="F18" s="16">
+        <f t="shared" si="0"/>
+        <v>1.2229257187890397</v>
+      </c>
+      <c r="G18" s="16">
+        <f t="shared" si="0"/>
+        <v>1.3077762259225187</v>
+      </c>
+      <c r="H18" s="16">
+        <f t="shared" si="0"/>
+        <v>1.3985139332760879</v>
+      </c>
+      <c r="I18" s="16">
+        <f t="shared" si="0"/>
+        <v>1.4955473136756892</v>
+      </c>
+      <c r="J18" s="16">
+        <f t="shared" si="0"/>
+        <v>1.5993131811015135</v>
+      </c>
+      <c r="K18" s="16">
+        <f t="shared" si="0"/>
+        <v>1.7102786570881465</v>
+      </c>
+      <c r="L18" s="16">
+        <f t="shared" si="0"/>
+        <v>1.8289432735598592</v>
+      </c>
+      <c r="M18" s="17">
+        <f t="shared" si="0"/>
+        <v>1.9558412215673537</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B19" s="25"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="19">
+        <f t="shared" ref="D19:M23" si="1">C18*(1+$C$11)</f>
+        <v>0.93511848170077816</v>
+      </c>
+      <c r="E19" s="19">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F19" s="19">
+        <f t="shared" si="1"/>
+        <v>1.0693832060523671</v>
+      </c>
+      <c r="G19" s="19">
+        <f t="shared" si="1"/>
+        <v>1.1435804413868396</v>
+      </c>
+      <c r="H19" s="19">
+        <f t="shared" si="1"/>
+        <v>1.2229257187890397</v>
+      </c>
+      <c r="I19" s="19">
+        <f t="shared" si="1"/>
+        <v>1.3077762259225187</v>
+      </c>
+      <c r="J19" s="19">
+        <f t="shared" si="1"/>
+        <v>1.3985139332760879</v>
+      </c>
+      <c r="K19" s="19">
+        <f t="shared" si="1"/>
+        <v>1.4955473136756889</v>
+      </c>
+      <c r="L19" s="19">
+        <f t="shared" si="1"/>
+        <v>1.5993131811015133</v>
+      </c>
+      <c r="M19" s="20">
+        <f t="shared" si="1"/>
+        <v>1.7102786570881465</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B20" s="25"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19">
+        <f t="shared" si="1"/>
+        <v>0.87444657481836863</v>
+      </c>
+      <c r="F20" s="19">
+        <f t="shared" si="1"/>
+        <v>0.93511848170077816</v>
+      </c>
+      <c r="G20" s="19">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H20" s="19">
+        <f t="shared" si="1"/>
+        <v>1.0693832060523671</v>
+      </c>
+      <c r="I20" s="19">
+        <f t="shared" si="1"/>
+        <v>1.1435804413868396</v>
+      </c>
+      <c r="J20" s="19">
+        <f t="shared" si="1"/>
+        <v>1.2229257187890397</v>
+      </c>
+      <c r="K20" s="19">
+        <f t="shared" si="1"/>
+        <v>1.3077762259225187</v>
+      </c>
+      <c r="L20" s="19">
+        <f t="shared" si="1"/>
+        <v>1.3985139332760876</v>
+      </c>
+      <c r="M20" s="20">
+        <f t="shared" si="1"/>
+        <v>1.4955473136756887</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B21" s="25"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19">
+        <f t="shared" si="1"/>
+        <v>0.81771115337259881</v>
+      </c>
+      <c r="G21" s="19">
+        <f t="shared" si="1"/>
+        <v>0.87444657481836863</v>
+      </c>
+      <c r="H21" s="19">
+        <f t="shared" si="1"/>
+        <v>0.93511848170077816</v>
+      </c>
+      <c r="I21" s="19">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J21" s="19">
+        <f t="shared" si="1"/>
+        <v>1.0693832060523671</v>
+      </c>
+      <c r="K21" s="19">
+        <f t="shared" si="1"/>
+        <v>1.1435804413868396</v>
+      </c>
+      <c r="L21" s="19">
+        <f t="shared" si="1"/>
+        <v>1.2229257187890397</v>
+      </c>
+      <c r="M21" s="20">
+        <f t="shared" si="1"/>
+        <v>1.3077762259225185</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B22" s="25"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19">
+        <f t="shared" si="1"/>
+        <v>0.76465681221157678</v>
+      </c>
+      <c r="H22" s="19">
+        <f t="shared" si="1"/>
+        <v>0.81771115337259881</v>
+      </c>
+      <c r="I22" s="19">
+        <f t="shared" si="1"/>
+        <v>0.87444657481836863</v>
+      </c>
+      <c r="J22" s="19">
+        <f t="shared" si="1"/>
+        <v>0.93511848170077816</v>
+      </c>
+      <c r="K22" s="19">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L22" s="19">
+        <f t="shared" si="1"/>
+        <v>1.0693832060523671</v>
+      </c>
+      <c r="M22" s="20">
+        <f t="shared" si="1"/>
+        <v>1.1435804413868396</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B23" s="25"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19">
+        <f t="shared" si="1"/>
+        <v>0.71504471725744667</v>
+      </c>
+      <c r="I23" s="19">
+        <f t="shared" si="1"/>
+        <v>0.76465681221157678</v>
+      </c>
+      <c r="J23" s="19">
+        <f t="shared" si="1"/>
+        <v>0.81771115337259881</v>
+      </c>
+      <c r="K23" s="19">
+        <f t="shared" si="1"/>
+        <v>0.87444657481836863</v>
+      </c>
+      <c r="L23" s="19">
+        <f t="shared" si="1"/>
+        <v>0.93511848170077816</v>
+      </c>
+      <c r="M23" s="20">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="R23" s="31"/>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B24" s="25"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19">
+        <f>H23*(1+$C$11)</f>
+        <v>0.66865153034994573</v>
+      </c>
+      <c r="J24" s="19">
+        <f>I23*(1+$C$11)</f>
+        <v>0.71504471725744667</v>
+      </c>
+      <c r="K24" s="19">
+        <f>J23*(1+$C$11)</f>
+        <v>0.76465681221157678</v>
+      </c>
+      <c r="L24" s="19">
+        <f>K23*(1+$C$11)</f>
+        <v>0.81771115337259881</v>
+      </c>
+      <c r="M24" s="20">
+        <f>L23*(1+$C$11)</f>
+        <v>0.87444657481836863</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B25" s="25"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19">
+        <f>I24*(1+$C$11)</f>
+        <v>0.62526840384774307</v>
+      </c>
+      <c r="K25" s="19">
+        <f>J24*(1+$C$11)</f>
+        <v>0.66865153034994573</v>
+      </c>
+      <c r="L25" s="19">
+        <f>K24*(1+$C$11)</f>
+        <v>0.71504471725744667</v>
+      </c>
+      <c r="M25" s="20">
+        <f>L24*(1+$C$11)</f>
+        <v>0.76465681221157678</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B26" s="25"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19">
+        <f>J25*(1+$C$11)</f>
+        <v>0.58470004046157054</v>
+      </c>
+      <c r="L26" s="19">
+        <f>K25*(1+$C$11)</f>
+        <v>0.62526840384774307</v>
+      </c>
+      <c r="M26" s="20">
+        <f>L25*(1+$C$11)</f>
+        <v>0.66865153034994573</v>
+      </c>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B27" s="25"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="19">
+        <f>K26*(1+$C$11)</f>
+        <v>0.54676381408680741</v>
+      </c>
+      <c r="M27" s="20">
+        <f>L26*(1+$C$11)</f>
+        <v>0.58470004046157054</v>
+      </c>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B28" s="26"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="22"/>
+      <c r="M28" s="23">
+        <f>L27*(1+$C$11)</f>
+        <v>0.51128894767778188</v>
+      </c>
+    </row>
+    <row r="30" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="3">
+        <v>-1</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B31" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B32" s="29"/>
+      <c r="C32" s="30"/>
+      <c r="G32" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B33" s="32"/>
+      <c r="C33" s="30"/>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B34" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="15">
+        <f t="shared" ref="C34:M39" si="2">MAX($C$30*(C18-$C$31),0)/(1+$C$9)^C$16</f>
+        <v>0</v>
+      </c>
+      <c r="D34" s="16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="17"/>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B35" s="25"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="19">
+        <f t="shared" si="2"/>
+        <v>6.4493394724520633E-2</v>
+      </c>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="20"/>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B36" s="25"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="19"/>
+      <c r="L36" s="19"/>
+      <c r="M36" s="20"/>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B37" s="25"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
+      <c r="L37" s="19"/>
+      <c r="M37" s="20"/>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B38" s="25"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="19"/>
+      <c r="K38" s="19"/>
+      <c r="L38" s="19"/>
+      <c r="M38" s="20"/>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B39" s="25"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
+      <c r="L39" s="19"/>
+      <c r="M39" s="20"/>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B40" s="25"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="19"/>
+      <c r="L40" s="19"/>
+      <c r="M40" s="20"/>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B41" s="25"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="19"/>
+      <c r="L41" s="19"/>
+      <c r="M41" s="20"/>
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B42" s="25"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="19"/>
+      <c r="K42" s="19"/>
+      <c r="L42" s="19"/>
+      <c r="M42" s="20"/>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B43" s="25"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="19"/>
+      <c r="K43" s="19"/>
+      <c r="L43" s="19"/>
+      <c r="M43" s="20"/>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B44" s="26"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="22"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
+      <c r="K44" s="22"/>
+      <c r="L44" s="22"/>
+      <c r="M44" s="23"/>
+    </row>
+    <row r="46" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G46" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B48" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" s="15"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="16"/>
+      <c r="H48" s="16"/>
+      <c r="I48" s="16"/>
+      <c r="J48" s="16"/>
+      <c r="K48" s="16"/>
+      <c r="L48" s="16">
+        <f t="shared" ref="C48:L57" si="3">MAX($C$12*M48+(1-$C$12)*M49,L34)</f>
+        <v>0</v>
+      </c>
+      <c r="M48" s="17">
+        <f>M34</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B49" s="25"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="19"/>
+      <c r="H49" s="19"/>
+      <c r="I49" s="19"/>
+      <c r="J49" s="19"/>
+      <c r="K49" s="19"/>
+      <c r="L49" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M49" s="20">
+        <f t="shared" ref="M49:M58" si="4">M35</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B50" s="25"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="19"/>
+      <c r="I50" s="19"/>
+      <c r="J50" s="19"/>
+      <c r="K50" s="19"/>
+      <c r="L50" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M50" s="20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B51" s="25"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="19"/>
+      <c r="G51" s="19"/>
+      <c r="H51" s="19"/>
+      <c r="I51" s="19"/>
+      <c r="J51" s="19"/>
+      <c r="K51" s="19"/>
+      <c r="L51" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M51" s="20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B52" s="25"/>
+      <c r="C52" s="18"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="19"/>
+      <c r="G52" s="19"/>
+      <c r="H52" s="19"/>
+      <c r="I52" s="19"/>
+      <c r="J52" s="19"/>
+      <c r="K52" s="19"/>
+      <c r="L52" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M52" s="20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B53" s="25"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="19"/>
+      <c r="F53" s="19"/>
+      <c r="G53" s="19"/>
+      <c r="H53" s="19"/>
+      <c r="I53" s="19"/>
+      <c r="J53" s="19"/>
+      <c r="K53" s="19"/>
+      <c r="L53" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M53" s="20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B54" s="25"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="19"/>
+      <c r="F54" s="19"/>
+      <c r="G54" s="19"/>
+      <c r="H54" s="19"/>
+      <c r="I54" s="19"/>
+      <c r="J54" s="19"/>
+      <c r="K54" s="19"/>
+      <c r="L54" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M54" s="20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B55" s="25"/>
+      <c r="C55" s="18"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="19"/>
+      <c r="F55" s="19"/>
+      <c r="G55" s="19"/>
+      <c r="H55" s="19"/>
+      <c r="I55" s="19"/>
+      <c r="J55" s="19"/>
+      <c r="K55" s="19"/>
+      <c r="L55" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M55" s="20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B56" s="25"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="19"/>
+      <c r="E56" s="19"/>
+      <c r="F56" s="19"/>
+      <c r="G56" s="19"/>
+      <c r="H56" s="19"/>
+      <c r="I56" s="19"/>
+      <c r="J56" s="19"/>
+      <c r="K56" s="19"/>
+      <c r="L56" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M56" s="20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B57" s="25"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="19"/>
+      <c r="F57" s="19"/>
+      <c r="G57" s="19"/>
+      <c r="H57" s="19"/>
+      <c r="I57" s="19"/>
+      <c r="J57" s="19"/>
+      <c r="K57" s="19"/>
+      <c r="L57" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M57" s="20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B58" s="26"/>
+      <c r="C58" s="27"/>
+      <c r="D58" s="28"/>
+      <c r="E58" s="28"/>
+      <c r="F58" s="28"/>
+      <c r="G58" s="28"/>
+      <c r="H58" s="28"/>
+      <c r="I58" s="28"/>
+      <c r="J58" s="28"/>
+      <c r="K58" s="28"/>
+      <c r="L58" s="28"/>
+      <c r="M58" s="23">
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1896,30 +2815,55 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="fa7e5010-1311-4096-a344-326d1919664c">JFHTZT72FDVU-254938863-279</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="fa7e5010-1311-4096-a344-326d1919664c">
-      <Url>https://intranet.d-fine.de/intern/miscellaneous/TemplateFramework/_layouts/15/DocIdRedir.aspx?ID=JFHTZT72FDVU-254938863-279</Url>
-      <Description>JFHTZT72FDVU-254938863-279</Description>
-    </_dlc_DocIdUrl>
-    <_Version xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <Tools xmlns="255ceb00-0504-4451-971c-89cf8ee3ad27"/>
-    <Comments xmlns="255ceb00-0504-4451-971c-89cf8ee3ad27" xsi:nil="true"/>
-    <Document_x0020_Category xmlns="255ceb00-0504-4451-971c-89cf8ee3ad27"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100135AEE51B13C7A4784C7A6FB658DD0E0" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c2ccf66da846160ccad12796df698db1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fa7e5010-1311-4096-a344-326d1919664c" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns4="255ceb00-0504-4451-971c-89cf8ee3ad27" xmlns:ns5="953edb04-63dd-49ba-ad7b-e9d17e0e7f06" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cd9e9067e801230649229059a2f6238c" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
     <xsd:import namespace="fa7e5010-1311-4096-a344-326d1919664c"/>
@@ -2165,84 +3109,40 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="fa7e5010-1311-4096-a344-326d1919664c">JFHTZT72FDVU-254938863-279</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="fa7e5010-1311-4096-a344-326d1919664c">
+      <Url>https://intranet.d-fine.de/intern/miscellaneous/TemplateFramework/_layouts/15/DocIdRedir.aspx?ID=JFHTZT72FDVU-254938863-279</Url>
+      <Description>JFHTZT72FDVU-254938863-279</Description>
+    </_dlc_DocIdUrl>
+    <_Version xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Tools xmlns="255ceb00-0504-4451-971c-89cf8ee3ad27"/>
+    <Comments xmlns="255ceb00-0504-4451-971c-89cf8ee3ad27" xsi:nil="true"/>
+    <Document_x0020_Category xmlns="255ceb00-0504-4451-971c-89cf8ee3ad27"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB0B7321-043A-43C5-BAA4-E29877D5579D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27E0ED53-E837-41F7-A9C9-5E67E49390EA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7017BB2C-A3F1-4167-848C-B358A8DC1CB9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="fa7e5010-1311-4096-a344-326d1919664c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="255ceb00-0504-4451-971c-89cf8ee3ad27"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="953edb04-63dd-49ba-ad7b-e9d17e0e7f06"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF6E80A2-72F6-4920-8A44-B99818E21D00}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2263,10 +3163,29 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7017BB2C-A3F1-4167-848C-B358A8DC1CB9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="fa7e5010-1311-4096-a344-326d1919664c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="255ceb00-0504-4451-971c-89cf8ee3ad27"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="953edb04-63dd-49ba-ad7b-e9d17e0e7f06"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27E0ED53-E837-41F7-A9C9-5E67E49390EA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB0B7321-043A-43C5-BAA4-E29877D5579D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>